<commit_message>
Add Magic Details, Began Tutorial
</commit_message>
<xml_diff>
--- a/Game Info Character.xlsx
+++ b/Game Info Character.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="170">
   <si>
     <t>Weapon</t>
   </si>
@@ -277,9 +277,6 @@
     <t>When worn and hit by physical damage reduce Phy Def by 1 and increase speed by 13%.</t>
   </si>
   <si>
-    <t>When hit by Magic Damage increase Phy Def by 2 and reduce speed by 3%.</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -503,6 +500,39 @@
   </si>
   <si>
     <t>Undead Screech</t>
+  </si>
+  <si>
+    <t>Damage 5</t>
+  </si>
+  <si>
+    <t>Chorus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If in control of Risen Undead deals 3 extra damage. </t>
+  </si>
+  <si>
+    <t>Element Type</t>
+  </si>
+  <si>
+    <t>Shadow</t>
+  </si>
+  <si>
+    <t>Darkness</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Lightning</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>Ice</t>
+  </si>
+  <si>
+    <t>When hit by Magic Damage increase Phy Def by 2 and reduce speed by 20%.</t>
   </si>
 </sst>
 </file>
@@ -1175,238 +1205,283 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>85</v>
       </c>
-      <c r="C1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="C3" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>119</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" t="s">
+        <v>120</v>
+      </c>
+      <c r="L3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N3" t="s">
         <v>121</v>
       </c>
-      <c r="J3" t="s">
-        <v>136</v>
-      </c>
-      <c r="L3" t="s">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>123</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L5" t="s">
+        <v>135</v>
+      </c>
+      <c r="N5" t="s">
         <v>124</v>
       </c>
-      <c r="J5" t="s">
-        <v>136</v>
-      </c>
-      <c r="L5" t="s">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" t="s">
-        <v>126</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" t="s">
+        <v>126</v>
+      </c>
+      <c r="L7" t="s">
+        <v>136</v>
+      </c>
+      <c r="N7" t="s">
         <v>127</v>
       </c>
-      <c r="J7" t="s">
-        <v>137</v>
-      </c>
-      <c r="L7" t="s">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>129</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="H9" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" t="s">
+        <v>129</v>
+      </c>
+      <c r="L9" t="s">
+        <v>135</v>
+      </c>
+      <c r="N9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" t="s">
         <v>130</v>
-      </c>
-      <c r="J9" t="s">
-        <v>136</v>
-      </c>
-      <c r="L9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" t="s">
-        <v>131</v>
       </c>
       <c r="F11">
         <v>2</v>
       </c>
       <c r="H11" t="s">
+        <v>164</v>
+      </c>
+      <c r="J11" t="s">
+        <v>131</v>
+      </c>
+      <c r="L11" t="s">
+        <v>137</v>
+      </c>
+      <c r="N11" t="s">
         <v>132</v>
       </c>
-      <c r="J11" t="s">
-        <v>138</v>
-      </c>
-      <c r="L11" t="s">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>134</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="J13" t="s">
+        <v>134</v>
+      </c>
+      <c r="L13" t="s">
+        <v>138</v>
+      </c>
+      <c r="N13" t="s">
         <v>139</v>
       </c>
-      <c r="L13" t="s">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" t="s">
-        <v>141</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="H15" t="s">
+        <v>166</v>
+      </c>
+      <c r="J15" t="s">
+        <v>141</v>
+      </c>
+      <c r="L15" t="s">
         <v>142</v>
       </c>
-      <c r="J15" t="s">
+      <c r="N15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
         <v>143</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J16" t="s">
-        <v>144</v>
-      </c>
-      <c r="L16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>147</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="J18" t="s">
         <v>148</v>
       </c>
       <c r="L18" t="s">
+        <v>147</v>
+      </c>
+      <c r="N18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" t="s">
-        <v>151</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="H20" t="s">
+        <v>164</v>
+      </c>
+      <c r="J20" t="s">
+        <v>151</v>
+      </c>
+      <c r="L20" t="s">
+        <v>135</v>
+      </c>
+      <c r="N20" t="s">
         <v>152</v>
       </c>
-      <c r="J20" t="s">
-        <v>136</v>
-      </c>
-      <c r="L20" t="s">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>154</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="H22" t="s">
+        <v>167</v>
+      </c>
+      <c r="J22" t="s">
+        <v>154</v>
+      </c>
+      <c r="L22" t="s">
         <v>155</v>
       </c>
-      <c r="J22" t="s">
+      <c r="N22" t="s">
         <v>156</v>
       </c>
-      <c r="L22" t="s">
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L23" t="s">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>159</v>
       </c>
       <c r="F25">
         <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>168</v>
+      </c>
+      <c r="J25" t="s">
+        <v>159</v>
+      </c>
+      <c r="L25" t="s">
+        <v>160</v>
+      </c>
+      <c r="N25" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1418,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,7 +1621,7 @@
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="P12" t="s">
-        <v>84</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1566,13 +1641,13 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
         <v>61</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -1589,13 +1664,13 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J3">
         <v>7</v>
@@ -1604,26 +1679,26 @@
         <v>12</v>
       </c>
       <c r="P3" t="s">
+        <v>112</v>
+      </c>
+      <c r="S3" t="s">
         <v>113</v>
-      </c>
-      <c r="S3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J6">
         <v>4</v>
@@ -1632,31 +1707,31 @@
         <v>12</v>
       </c>
       <c r="P6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" t="s">
         <v>98</v>
-      </c>
-      <c r="F10" t="s">
-        <v>99</v>
       </c>
       <c r="J10">
         <v>6</v>
@@ -1665,26 +1740,26 @@
         <v>10</v>
       </c>
       <c r="P10" t="s">
+        <v>99</v>
+      </c>
+      <c r="S10" t="s">
         <v>100</v>
-      </c>
-      <c r="S10" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" t="s">
         <v>103</v>
-      </c>
-      <c r="F13" t="s">
-        <v>104</v>
       </c>
       <c r="J13">
         <v>5</v>
@@ -1693,21 +1768,21 @@
         <v>11</v>
       </c>
       <c r="P13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S13" t="s">
         <v>105</v>
-      </c>
-      <c r="S13" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" t="s">
         <v>107</v>
-      </c>
-      <c r="F15" t="s">
-        <v>108</v>
       </c>
       <c r="J15">
         <v>4</v>
@@ -1716,10 +1791,10 @@
         <v>13</v>
       </c>
       <c r="P15" t="s">
+        <v>108</v>
+      </c>
+      <c r="S15" t="s">
         <v>109</v>
-      </c>
-      <c r="S15" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>